<commit_message>
Update Cykle - prasy ML i DL V2.xlsx
</commit_message>
<xml_diff>
--- a/V2/Cykle - prasy ML i DL V2.xlsx
+++ b/V2/Cykle - prasy ML i DL V2.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>pojemność</t>
   </si>
@@ -135,10 +135,6 @@
 CYKL [s]</t>
   </si>
   <si>
-    <t>PRASY DL
-CYKL [s]</t>
-  </si>
-  <si>
     <t>*1,25</t>
   </si>
   <si>
@@ -147,6 +143,12 @@
   </si>
   <si>
     <t>V2</t>
+  </si>
+  <si>
+    <t>PRASY DL CYKL [s]</t>
+  </si>
+  <si>
+    <t>OEE 0,75</t>
   </si>
 </sst>
 </file>
@@ -862,87 +864,87 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -1297,44 +1299,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="47" t="s">
+      <c r="A1" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="60" t="s">
+      <c r="F1" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="47" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1">
-      <c r="A2" s="44"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="54"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="65"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="50"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="48"/>
     </row>
     <row r="3" spans="1:10" ht="14.45" customHeight="1">
       <c r="B3" s="17" t="s">
@@ -1343,23 +1345,23 @@
       <c r="C3" s="18">
         <v>140</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="54" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="29"/>
       <c r="G3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="66" t="str">
+        <v>33</v>
+      </c>
+      <c r="H3" s="40" t="str">
         <f>IF(B3="",H2, IF(ISNUMBER(FIND("-", B3)), LEFT(B3, FIND("-",B3)-1),B3))</f>
         <v>5</v>
       </c>
-      <c r="I3" s="67">
+      <c r="I3" s="41">
         <f>IF(C3="",I2,C3)</f>
         <v>140</v>
       </c>
-      <c r="J3" s="68" t="str">
+      <c r="J3" s="42" t="str">
         <f>IF(D3="",J2, IF(ISNUMBER(FIND("-", D3)), LEFT(D3, FIND("-",D3)-1),D3))</f>
         <v>2,45</v>
       </c>
@@ -1369,7 +1371,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="41"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="23">
         <v>70</v>
       </c>
@@ -1377,15 +1379,15 @@
         <f>E4*1.25</f>
         <v>87.5</v>
       </c>
-      <c r="H4" s="66" t="str">
+      <c r="H4" s="40" t="str">
         <f t="shared" ref="H4:H67" si="0">IF(B4="",H3, IF(ISNUMBER(FIND("-", B4)), LEFT(B4, FIND("-",B4)-1),B4))</f>
         <v>5</v>
       </c>
-      <c r="I4" s="67">
+      <c r="I4" s="41">
         <f t="shared" ref="I4:I67" si="1">IF(C4="",I3,C4)</f>
         <v>140</v>
       </c>
-      <c r="J4" s="68" t="str">
+      <c r="J4" s="42" t="str">
         <f t="shared" ref="J4:J67" si="2">IF(D4="",J3, IF(ISNUMBER(FIND("-", D4)), LEFT(D4, FIND("-",D4)-1),D4))</f>
         <v>2,45</v>
       </c>
@@ -1395,7 +1397,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="41"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="23">
         <v>72</v>
       </c>
@@ -1403,15 +1405,15 @@
         <f t="shared" ref="F5:F68" si="3">E5*1.25</f>
         <v>90</v>
       </c>
-      <c r="H5" s="66">
+      <c r="H5" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I5" s="67">
+      <c r="I5" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J5" s="68" t="str">
+      <c r="J5" s="42" t="str">
         <f t="shared" si="2"/>
         <v>2,45</v>
       </c>
@@ -1421,7 +1423,7 @@
         <v>13.4</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="42"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="23">
         <v>74</v>
       </c>
@@ -1429,15 +1431,15 @@
         <f t="shared" si="3"/>
         <v>92.5</v>
       </c>
-      <c r="H6" s="66">
+      <c r="H6" s="40">
         <f t="shared" si="0"/>
         <v>13.4</v>
       </c>
-      <c r="I6" s="67">
+      <c r="I6" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J6" s="68" t="str">
+      <c r="J6" s="42" t="str">
         <f t="shared" si="2"/>
         <v>2,45</v>
       </c>
@@ -1459,15 +1461,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H7" s="66" t="str">
+      <c r="H7" s="40" t="str">
         <f t="shared" si="0"/>
         <v>6elip</v>
       </c>
-      <c r="I7" s="67">
+      <c r="I7" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J7" s="68">
+      <c r="J7" s="42">
         <f t="shared" si="2"/>
         <v>2.7</v>
       </c>
@@ -1479,20 +1481,20 @@
       <c r="C8" s="3">
         <v>140</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="51" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="30"/>
-      <c r="H8" s="66" t="str">
+      <c r="H8" s="40" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I8" s="67">
+      <c r="I8" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J8" s="68" t="str">
+      <c r="J8" s="42" t="str">
         <f t="shared" si="2"/>
         <v>2,8</v>
       </c>
@@ -1502,7 +1504,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="41"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="23">
         <v>70</v>
       </c>
@@ -1510,15 +1512,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H9" s="66" t="str">
+      <c r="H9" s="40" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I9" s="67">
+      <c r="I9" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J9" s="68" t="str">
+      <c r="J9" s="42" t="str">
         <f t="shared" si="2"/>
         <v>2,8</v>
       </c>
@@ -1528,7 +1530,7 @@
         <v>7.5</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="41"/>
+      <c r="D10" s="52"/>
       <c r="E10" s="23">
         <v>70</v>
       </c>
@@ -1536,15 +1538,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="40">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="I10" s="67">
+      <c r="I10" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J10" s="68" t="str">
+      <c r="J10" s="42" t="str">
         <f t="shared" si="2"/>
         <v>2,8</v>
       </c>
@@ -1554,7 +1556,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="41"/>
+      <c r="D11" s="52"/>
       <c r="E11" s="23">
         <v>72</v>
       </c>
@@ -1562,15 +1564,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I11" s="67">
+      <c r="I11" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J11" s="68" t="str">
+      <c r="J11" s="42" t="str">
         <f t="shared" si="2"/>
         <v>2,8</v>
       </c>
@@ -1580,7 +1582,7 @@
         <v>13.4</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="42"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="23">
         <v>74</v>
       </c>
@@ -1588,15 +1590,15 @@
         <f t="shared" si="3"/>
         <v>92.5</v>
       </c>
-      <c r="H12" s="66">
+      <c r="H12" s="40">
         <f t="shared" si="0"/>
         <v>13.4</v>
       </c>
-      <c r="I12" s="67">
+      <c r="I12" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J12" s="68" t="str">
+      <c r="J12" s="42" t="str">
         <f t="shared" si="2"/>
         <v>2,8</v>
       </c>
@@ -1608,20 +1610,20 @@
       <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="51">
         <v>3.1</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="30"/>
-      <c r="H13" s="66" t="str">
+      <c r="H13" s="40" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I13" s="67" t="str">
+      <c r="I13" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J13" s="68">
+      <c r="J13" s="42">
         <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
@@ -1631,7 +1633,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="41"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="23">
         <v>70</v>
       </c>
@@ -1639,15 +1641,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H14" s="66" t="str">
+      <c r="H14" s="40" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I14" s="67" t="str">
+      <c r="I14" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J14" s="68">
+      <c r="J14" s="42">
         <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>6.7</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="41"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="23">
         <v>70</v>
       </c>
@@ -1665,15 +1667,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H15" s="66">
+      <c r="H15" s="40">
         <f t="shared" si="0"/>
         <v>6.7</v>
       </c>
-      <c r="I15" s="67" t="str">
+      <c r="I15" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J15" s="68">
+      <c r="J15" s="42">
         <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
@@ -1683,7 +1685,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="41"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="23">
         <v>70</v>
       </c>
@@ -1691,15 +1693,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H16" s="66">
+      <c r="H16" s="40">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I16" s="67" t="str">
+      <c r="I16" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J16" s="68">
+      <c r="J16" s="42">
         <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="41"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="23">
         <v>70</v>
       </c>
@@ -1717,15 +1719,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H17" s="66">
+      <c r="H17" s="40">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I17" s="67" t="str">
+      <c r="I17" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J17" s="68">
+      <c r="J17" s="42">
         <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
@@ -1735,7 +1737,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="41"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="23">
         <v>72</v>
       </c>
@@ -1743,15 +1745,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H18" s="66">
+      <c r="H18" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I18" s="67" t="str">
+      <c r="I18" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J18" s="68">
+      <c r="J18" s="42">
         <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
@@ -1761,7 +1763,7 @@
         <v>13.4</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="42"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="23">
         <v>74</v>
       </c>
@@ -1769,15 +1771,15 @@
         <f t="shared" si="3"/>
         <v>92.5</v>
       </c>
-      <c r="H19" s="66">
+      <c r="H19" s="40">
         <f t="shared" si="0"/>
         <v>13.4</v>
       </c>
-      <c r="I19" s="67" t="str">
+      <c r="I19" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J19" s="68">
+      <c r="J19" s="42">
         <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
@@ -1799,15 +1801,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H20" s="66">
+      <c r="H20" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I20" s="67">
+      <c r="I20" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J20" s="68">
+      <c r="J20" s="42">
         <f t="shared" si="2"/>
         <v>3.3</v>
       </c>
@@ -1819,20 +1821,20 @@
       <c r="C21" s="3">
         <v>140</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="51" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="30"/>
-      <c r="H21" s="66" t="str">
+      <c r="H21" s="40" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I21" s="67">
+      <c r="I21" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J21" s="68" t="str">
+      <c r="J21" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,4</v>
       </c>
@@ -1842,7 +1844,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="41"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="23">
         <v>70</v>
       </c>
@@ -1850,15 +1852,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H22" s="66">
+      <c r="H22" s="40">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I22" s="67">
+      <c r="I22" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J22" s="68" t="str">
+      <c r="J22" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,4</v>
       </c>
@@ -1868,7 +1870,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="41"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="23">
         <v>70</v>
       </c>
@@ -1876,15 +1878,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H23" s="66">
+      <c r="H23" s="40">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I23" s="67">
+      <c r="I23" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J23" s="68" t="str">
+      <c r="J23" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,4</v>
       </c>
@@ -1894,7 +1896,7 @@
         <v>10</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="42"/>
+      <c r="D24" s="53"/>
       <c r="E24" s="23">
         <v>72</v>
       </c>
@@ -1902,15 +1904,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H24" s="66">
+      <c r="H24" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I24" s="67">
+      <c r="I24" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J24" s="68" t="str">
+      <c r="J24" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,4</v>
       </c>
@@ -1932,15 +1934,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H25" s="66" t="str">
+      <c r="H25" s="40" t="str">
         <f t="shared" si="0"/>
         <v>6,8elip</v>
       </c>
-      <c r="I25" s="67" t="str">
+      <c r="I25" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J25" s="68">
+      <c r="J25" s="42">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
@@ -1952,20 +1954,20 @@
       <c r="C26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="51" t="s">
         <v>30</v>
       </c>
       <c r="E26" s="24"/>
       <c r="F26" s="30"/>
-      <c r="H26" s="66" t="str">
+      <c r="H26" s="40" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I26" s="67" t="str">
+      <c r="I26" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J26" s="68" t="str">
+      <c r="J26" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -1975,7 +1977,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="41"/>
+      <c r="D27" s="52"/>
       <c r="E27" s="23">
         <v>70</v>
       </c>
@@ -1983,15 +1985,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H27" s="66">
+      <c r="H27" s="40">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I27" s="67" t="str">
+      <c r="I27" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J27" s="68" t="str">
+      <c r="J27" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -2001,7 +2003,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="41"/>
+      <c r="D28" s="52"/>
       <c r="E28" s="23">
         <v>70</v>
       </c>
@@ -2009,15 +2011,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H28" s="66">
+      <c r="H28" s="40">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I28" s="67" t="str">
+      <c r="I28" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J28" s="68" t="str">
+      <c r="J28" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -2027,7 +2029,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="41"/>
+      <c r="D29" s="52"/>
       <c r="E29" s="23">
         <v>70</v>
       </c>
@@ -2035,15 +2037,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H29" s="66">
+      <c r="H29" s="40">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I29" s="67" t="str">
+      <c r="I29" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J29" s="68" t="str">
+      <c r="J29" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -2053,7 +2055,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="42"/>
+      <c r="D30" s="53"/>
       <c r="E30" s="23">
         <v>74</v>
       </c>
@@ -2061,15 +2063,15 @@
         <f t="shared" si="3"/>
         <v>92.5</v>
       </c>
-      <c r="H30" s="66">
+      <c r="H30" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I30" s="67" t="str">
+      <c r="I30" s="41" t="str">
         <f t="shared" si="1"/>
         <v>140-141</v>
       </c>
-      <c r="J30" s="68" t="str">
+      <c r="J30" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -2081,7 +2083,7 @@
       <c r="C31" s="3">
         <v>140</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="51">
         <v>3.95</v>
       </c>
       <c r="E31" s="24"/>
@@ -2089,15 +2091,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H31" s="66" t="str">
+      <c r="H31" s="40" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I31" s="67">
+      <c r="I31" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J31" s="68">
+      <c r="J31" s="42">
         <f t="shared" si="2"/>
         <v>3.95</v>
       </c>
@@ -2107,7 +2109,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="41"/>
+      <c r="D32" s="52"/>
       <c r="E32" s="23">
         <v>70</v>
       </c>
@@ -2115,15 +2117,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H32" s="66">
+      <c r="H32" s="40">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I32" s="67">
+      <c r="I32" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J32" s="68">
+      <c r="J32" s="42">
         <f t="shared" si="2"/>
         <v>3.95</v>
       </c>
@@ -2133,7 +2135,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="D33" s="41"/>
+      <c r="D33" s="52"/>
       <c r="E33" s="23">
         <v>70</v>
       </c>
@@ -2141,15 +2143,15 @@
         <f t="shared" si="3"/>
         <v>87.5</v>
       </c>
-      <c r="H33" s="66">
+      <c r="H33" s="40">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I33" s="67">
+      <c r="I33" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J33" s="68">
+      <c r="J33" s="42">
         <f t="shared" si="2"/>
         <v>3.95</v>
       </c>
@@ -2159,7 +2161,7 @@
         <v>10</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="46"/>
+      <c r="D34" s="55"/>
       <c r="E34" s="25">
         <v>74</v>
       </c>
@@ -2167,15 +2169,15 @@
         <f t="shared" si="3"/>
         <v>92.5</v>
       </c>
-      <c r="H34" s="66">
+      <c r="H34" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I34" s="67">
+      <c r="I34" s="41">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="J34" s="68">
+      <c r="J34" s="42">
         <f t="shared" si="2"/>
         <v>3.95</v>
       </c>
@@ -2197,15 +2199,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H35" s="66">
+      <c r="H35" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I35" s="67">
+      <c r="I35" s="41">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="J35" s="68">
+      <c r="J35" s="42">
         <f t="shared" si="2"/>
         <v>2.8</v>
       </c>
@@ -2217,20 +2219,20 @@
       <c r="C36" s="3">
         <v>160</v>
       </c>
-      <c r="D36" s="40">
+      <c r="D36" s="51">
         <v>3.4</v>
       </c>
       <c r="E36" s="23"/>
       <c r="F36" s="30"/>
-      <c r="H36" s="66" t="str">
+      <c r="H36" s="40" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I36" s="67">
+      <c r="I36" s="41">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="J36" s="68">
+      <c r="J36" s="42">
         <f t="shared" si="2"/>
         <v>3.4</v>
       </c>
@@ -2240,7 +2242,7 @@
         <v>10</v>
       </c>
       <c r="C37" s="3"/>
-      <c r="D37" s="41"/>
+      <c r="D37" s="52"/>
       <c r="E37" s="23">
         <v>72</v>
       </c>
@@ -2248,15 +2250,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H37" s="66">
+      <c r="H37" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I37" s="67">
+      <c r="I37" s="41">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="J37" s="68">
+      <c r="J37" s="42">
         <f t="shared" si="2"/>
         <v>3.4</v>
       </c>
@@ -2266,7 +2268,7 @@
         <v>14</v>
       </c>
       <c r="C38" s="3"/>
-      <c r="D38" s="42"/>
+      <c r="D38" s="53"/>
       <c r="E38" s="23">
         <v>74</v>
       </c>
@@ -2274,15 +2276,15 @@
         <f t="shared" si="3"/>
         <v>92.5</v>
       </c>
-      <c r="H38" s="66">
+      <c r="H38" s="40">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="I38" s="67">
+      <c r="I38" s="41">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="J38" s="68">
+      <c r="J38" s="42">
         <f t="shared" si="2"/>
         <v>3.4</v>
       </c>
@@ -2304,15 +2306,15 @@
         <f t="shared" si="3"/>
         <v>92.5</v>
       </c>
-      <c r="H39" s="66">
+      <c r="H39" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I39" s="67">
+      <c r="I39" s="41">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="J39" s="68" t="str">
+      <c r="J39" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,9</v>
       </c>
@@ -2324,20 +2326,20 @@
       <c r="C40" s="18">
         <v>171</v>
       </c>
-      <c r="D40" s="45">
+      <c r="D40" s="54">
         <v>3.45</v>
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="29"/>
-      <c r="H40" s="66" t="str">
+      <c r="H40" s="40" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I40" s="67">
+      <c r="I40" s="41">
         <f t="shared" si="1"/>
         <v>171</v>
       </c>
-      <c r="J40" s="68">
+      <c r="J40" s="42">
         <f t="shared" si="2"/>
         <v>3.45</v>
       </c>
@@ -2347,7 +2349,7 @@
         <v>10</v>
       </c>
       <c r="C41" s="3"/>
-      <c r="D41" s="42"/>
+      <c r="D41" s="53"/>
       <c r="E41" s="23">
         <v>72</v>
       </c>
@@ -2355,15 +2357,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H41" s="66">
+      <c r="H41" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I41" s="67">
+      <c r="I41" s="41">
         <f t="shared" si="1"/>
         <v>171</v>
       </c>
-      <c r="J41" s="68">
+      <c r="J41" s="42">
         <f t="shared" si="2"/>
         <v>3.45</v>
       </c>
@@ -2375,20 +2377,20 @@
       <c r="C42" s="3">
         <v>171</v>
       </c>
-      <c r="D42" s="40">
+      <c r="D42" s="51">
         <v>3.6</v>
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="30"/>
-      <c r="H42" s="66" t="str">
+      <c r="H42" s="40" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I42" s="67">
+      <c r="I42" s="41">
         <f t="shared" si="1"/>
         <v>171</v>
       </c>
-      <c r="J42" s="68">
+      <c r="J42" s="42">
         <f t="shared" si="2"/>
         <v>3.6</v>
       </c>
@@ -2398,7 +2400,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="4"/>
-      <c r="D43" s="46"/>
+      <c r="D43" s="55"/>
       <c r="E43" s="25">
         <v>72</v>
       </c>
@@ -2406,15 +2408,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H43" s="66">
+      <c r="H43" s="40">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I43" s="67">
+      <c r="I43" s="41">
         <f t="shared" si="1"/>
         <v>171</v>
       </c>
-      <c r="J43" s="68">
+      <c r="J43" s="42">
         <f t="shared" si="2"/>
         <v>3.6</v>
       </c>
@@ -2426,20 +2428,20 @@
       <c r="C44" s="5">
         <v>178</v>
       </c>
-      <c r="D44" s="41">
+      <c r="D44" s="52">
         <v>3.1</v>
       </c>
       <c r="E44" s="26"/>
       <c r="F44" s="29"/>
-      <c r="H44" s="66" t="str">
+      <c r="H44" s="40" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I44" s="67">
+      <c r="I44" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J44" s="68">
+      <c r="J44" s="42">
         <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
@@ -2449,7 +2451,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="3"/>
-      <c r="D45" s="42"/>
+      <c r="D45" s="53"/>
       <c r="E45" s="23">
         <v>72</v>
       </c>
@@ -2457,15 +2459,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H45" s="66">
+      <c r="H45" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I45" s="67">
+      <c r="I45" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J45" s="68">
+      <c r="J45" s="42">
         <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
@@ -2477,20 +2479,20 @@
       <c r="C46" s="3">
         <v>178</v>
       </c>
-      <c r="D46" s="40">
+      <c r="D46" s="51">
         <v>3.2</v>
       </c>
       <c r="E46" s="23"/>
       <c r="F46" s="30"/>
-      <c r="H46" s="66" t="str">
+      <c r="H46" s="40" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I46" s="67">
+      <c r="I46" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J46" s="68">
+      <c r="J46" s="42">
         <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
@@ -2500,7 +2502,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="3"/>
-      <c r="D47" s="41"/>
+      <c r="D47" s="52"/>
       <c r="E47" s="23">
         <v>72</v>
       </c>
@@ -2508,15 +2510,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H47" s="66">
+      <c r="H47" s="40">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I47" s="67">
+      <c r="I47" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J47" s="68">
+      <c r="J47" s="42">
         <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
@@ -2526,7 +2528,7 @@
         <v>10</v>
       </c>
       <c r="C48" s="3"/>
-      <c r="D48" s="41"/>
+      <c r="D48" s="52"/>
       <c r="E48" s="23">
         <v>72</v>
       </c>
@@ -2534,15 +2536,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H48" s="66">
+      <c r="H48" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I48" s="67">
+      <c r="I48" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J48" s="68">
+      <c r="J48" s="42">
         <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
@@ -2552,7 +2554,7 @@
         <v>11</v>
       </c>
       <c r="C49" s="3"/>
-      <c r="D49" s="42"/>
+      <c r="D49" s="53"/>
       <c r="E49" s="23">
         <v>72</v>
       </c>
@@ -2560,15 +2562,15 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H49" s="66">
+      <c r="H49" s="40">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="I49" s="67">
+      <c r="I49" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J49" s="68">
+      <c r="J49" s="42">
         <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
@@ -2580,20 +2582,20 @@
       <c r="C50" s="3">
         <v>178</v>
       </c>
-      <c r="D50" s="40">
+      <c r="D50" s="51">
         <v>3.6</v>
       </c>
       <c r="E50" s="23"/>
       <c r="F50" s="30"/>
-      <c r="H50" s="66" t="str">
+      <c r="H50" s="40" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I50" s="67">
+      <c r="I50" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J50" s="68">
+      <c r="J50" s="42">
         <f t="shared" si="2"/>
         <v>3.6</v>
       </c>
@@ -2603,7 +2605,7 @@
         <v>8</v>
       </c>
       <c r="C51" s="3"/>
-      <c r="D51" s="42"/>
+      <c r="D51" s="53"/>
       <c r="E51" s="23">
         <v>74</v>
       </c>
@@ -2611,15 +2613,15 @@
         <f t="shared" si="3"/>
         <v>92.5</v>
       </c>
-      <c r="H51" s="66">
+      <c r="H51" s="40">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I51" s="67">
+      <c r="I51" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J51" s="68">
+      <c r="J51" s="42">
         <f t="shared" si="2"/>
         <v>3.6</v>
       </c>
@@ -2631,20 +2633,20 @@
       <c r="C52" s="3">
         <v>178</v>
       </c>
-      <c r="D52" s="40" t="s">
+      <c r="D52" s="51" t="s">
         <v>24</v>
       </c>
       <c r="E52" s="23"/>
       <c r="F52" s="30"/>
-      <c r="H52" s="66" t="str">
+      <c r="H52" s="40" t="str">
         <f t="shared" si="0"/>
         <v>8,3</v>
       </c>
-      <c r="I52" s="67">
+      <c r="I52" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J52" s="68" t="str">
+      <c r="J52" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -2654,7 +2656,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="C53" s="3"/>
-      <c r="D53" s="41"/>
+      <c r="D53" s="52"/>
       <c r="E53" s="23">
         <v>76</v>
       </c>
@@ -2662,15 +2664,15 @@
         <f t="shared" si="3"/>
         <v>95</v>
       </c>
-      <c r="H53" s="66">
+      <c r="H53" s="40">
         <f t="shared" si="0"/>
         <v>8.3000000000000007</v>
       </c>
-      <c r="I53" s="67">
+      <c r="I53" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J53" s="68" t="str">
+      <c r="J53" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -2680,7 +2682,7 @@
         <v>10.8</v>
       </c>
       <c r="C54" s="3"/>
-      <c r="D54" s="41"/>
+      <c r="D54" s="52"/>
       <c r="E54" s="23">
         <v>78</v>
       </c>
@@ -2688,15 +2690,15 @@
         <f t="shared" si="3"/>
         <v>97.5</v>
       </c>
-      <c r="H54" s="66">
+      <c r="H54" s="40">
         <f t="shared" si="0"/>
         <v>10.8</v>
       </c>
-      <c r="I54" s="67">
+      <c r="I54" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J54" s="68" t="str">
+      <c r="J54" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -2706,7 +2708,7 @@
         <v>14</v>
       </c>
       <c r="C55" s="3"/>
-      <c r="D55" s="41"/>
+      <c r="D55" s="52"/>
       <c r="E55" s="23">
         <v>79</v>
       </c>
@@ -2714,15 +2716,15 @@
         <f t="shared" si="3"/>
         <v>98.75</v>
       </c>
-      <c r="H55" s="66">
+      <c r="H55" s="40">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="I55" s="67">
+      <c r="I55" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J55" s="68" t="str">
+      <c r="J55" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -2732,7 +2734,7 @@
         <v>15.75</v>
       </c>
       <c r="C56" s="3"/>
-      <c r="D56" s="42"/>
+      <c r="D56" s="53"/>
       <c r="E56" s="23">
         <v>82</v>
       </c>
@@ -2740,15 +2742,15 @@
         <f t="shared" si="3"/>
         <v>102.5</v>
       </c>
-      <c r="H56" s="66">
+      <c r="H56" s="40">
         <f t="shared" si="0"/>
         <v>15.75</v>
       </c>
-      <c r="I56" s="67">
+      <c r="I56" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J56" s="68" t="str">
+      <c r="J56" s="42" t="str">
         <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
@@ -2770,15 +2772,15 @@
         <f t="shared" si="3"/>
         <v>98.75</v>
       </c>
-      <c r="H57" s="66" t="str">
+      <c r="H57" s="40" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I57" s="67">
+      <c r="I57" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J57" s="68">
+      <c r="J57" s="42">
         <f t="shared" si="2"/>
         <v>4.4000000000000004</v>
       </c>
@@ -2790,20 +2792,20 @@
       <c r="C58" s="3">
         <v>178</v>
       </c>
-      <c r="D58" s="40">
+      <c r="D58" s="51">
         <v>4.6500000000000004</v>
       </c>
       <c r="E58" s="23"/>
       <c r="F58" s="30"/>
-      <c r="H58" s="66" t="str">
+      <c r="H58" s="40" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I58" s="67">
+      <c r="I58" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J58" s="68">
+      <c r="J58" s="42">
         <f t="shared" si="2"/>
         <v>4.6500000000000004</v>
       </c>
@@ -2813,7 +2815,7 @@
         <v>12</v>
       </c>
       <c r="C59" s="3"/>
-      <c r="D59" s="42"/>
+      <c r="D59" s="53"/>
       <c r="E59" s="23">
         <v>80</v>
       </c>
@@ -2821,15 +2823,15 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="H59" s="66">
+      <c r="H59" s="40">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="I59" s="67">
+      <c r="I59" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J59" s="68">
+      <c r="J59" s="42">
         <f t="shared" si="2"/>
         <v>4.6500000000000004</v>
       </c>
@@ -2846,15 +2848,15 @@
       </c>
       <c r="E60" s="23"/>
       <c r="F60" s="30"/>
-      <c r="H60" s="66" t="str">
+      <c r="H60" s="40" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I60" s="67">
+      <c r="I60" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J60" s="68">
+      <c r="J60" s="42">
         <f t="shared" si="2"/>
         <v>4.8</v>
       </c>
@@ -2876,15 +2878,15 @@
         <f t="shared" si="3"/>
         <v>106.25</v>
       </c>
-      <c r="H61" s="66" t="str">
+      <c r="H61" s="40" t="str">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="I61" s="67">
+      <c r="I61" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J61" s="68">
+      <c r="J61" s="42">
         <f t="shared" si="2"/>
         <v>4.9000000000000004</v>
       </c>
@@ -2896,20 +2898,20 @@
       <c r="C62" s="3">
         <v>178</v>
       </c>
-      <c r="D62" s="40">
+      <c r="D62" s="51">
         <v>6.7</v>
       </c>
       <c r="E62" s="23"/>
       <c r="F62" s="30"/>
-      <c r="H62" s="66" t="str">
+      <c r="H62" s="40" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I62" s="67">
+      <c r="I62" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J62" s="68">
+      <c r="J62" s="42">
         <f t="shared" si="2"/>
         <v>6.7</v>
       </c>
@@ -2919,7 +2921,7 @@
         <v>10</v>
       </c>
       <c r="C63" s="12"/>
-      <c r="D63" s="41"/>
+      <c r="D63" s="52"/>
       <c r="E63" s="27">
         <v>88</v>
       </c>
@@ -2927,15 +2929,15 @@
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="H63" s="66">
+      <c r="H63" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I63" s="67">
+      <c r="I63" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J63" s="68">
+      <c r="J63" s="42">
         <f t="shared" si="2"/>
         <v>6.7</v>
       </c>
@@ -2945,7 +2947,7 @@
         <v>15</v>
       </c>
       <c r="C64" s="12"/>
-      <c r="D64" s="41"/>
+      <c r="D64" s="52"/>
       <c r="E64" s="27">
         <v>90</v>
       </c>
@@ -2953,15 +2955,15 @@
         <f t="shared" si="3"/>
         <v>112.5</v>
       </c>
-      <c r="H64" s="66">
+      <c r="H64" s="40">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="I64" s="67">
+      <c r="I64" s="41">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="J64" s="68">
+      <c r="J64" s="42">
         <f t="shared" si="2"/>
         <v>6.7</v>
       </c>
@@ -2983,15 +2985,15 @@
         <f t="shared" si="3"/>
         <v>107.5</v>
       </c>
-      <c r="H65" s="66" t="str">
+      <c r="H65" s="40" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="I65" s="67">
+      <c r="I65" s="41">
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
-      <c r="J65" s="68">
+      <c r="J65" s="42">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
@@ -3013,15 +3015,15 @@
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="H66" s="66" t="str">
+      <c r="H66" s="40" t="str">
         <f t="shared" si="0"/>
         <v>13,4</v>
       </c>
-      <c r="I66" s="67">
+      <c r="I66" s="41">
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
-      <c r="J66" s="68">
+      <c r="J66" s="42">
         <f t="shared" si="2"/>
         <v>3.4</v>
       </c>
@@ -3033,20 +3035,20 @@
       <c r="C67" s="3">
         <v>204</v>
       </c>
-      <c r="D67" s="40">
+      <c r="D67" s="51">
         <v>3.6</v>
       </c>
       <c r="E67" s="24"/>
       <c r="F67" s="30"/>
-      <c r="H67" s="66" t="str">
+      <c r="H67" s="40" t="str">
         <f t="shared" si="0"/>
         <v>10,7</v>
       </c>
-      <c r="I67" s="67">
+      <c r="I67" s="41">
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
-      <c r="J67" s="68">
+      <c r="J67" s="42">
         <f t="shared" si="2"/>
         <v>3.6</v>
       </c>
@@ -3056,7 +3058,7 @@
         <v>13.4</v>
       </c>
       <c r="C68" s="3"/>
-      <c r="D68" s="41"/>
+      <c r="D68" s="52"/>
       <c r="E68" s="23">
         <v>88</v>
       </c>
@@ -3064,15 +3066,15 @@
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="H68" s="66">
+      <c r="H68" s="40">
         <f t="shared" ref="H68:H77" si="4">IF(B68="",H67, IF(ISNUMBER(FIND("-", B68)), LEFT(B68, FIND("-",B68)-1),B68))</f>
         <v>13.4</v>
       </c>
-      <c r="I68" s="67">
+      <c r="I68" s="41">
         <f t="shared" ref="I68:I77" si="5">IF(C68="",I67,C68)</f>
         <v>204</v>
       </c>
-      <c r="J68" s="68">
+      <c r="J68" s="42">
         <f t="shared" ref="J68:J77" si="6">IF(D68="",J67, IF(ISNUMBER(FIND("-", D68)), LEFT(D68, FIND("-",D68)-1),D68))</f>
         <v>3.6</v>
       </c>
@@ -3082,7 +3084,7 @@
         <v>20</v>
       </c>
       <c r="C69" s="3"/>
-      <c r="D69" s="42"/>
+      <c r="D69" s="53"/>
       <c r="E69" s="23">
         <v>90</v>
       </c>
@@ -3090,15 +3092,15 @@
         <f t="shared" ref="F69:F77" si="7">E69*1.25</f>
         <v>112.5</v>
       </c>
-      <c r="H69" s="66">
+      <c r="H69" s="40">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="I69" s="67">
+      <c r="I69" s="41">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
-      <c r="J69" s="68">
+      <c r="J69" s="42">
         <f t="shared" si="6"/>
         <v>3.6</v>
       </c>
@@ -3110,20 +3112,20 @@
       <c r="C70" s="3">
         <v>204</v>
       </c>
-      <c r="D70" s="40">
+      <c r="D70" s="51">
         <v>3.8</v>
       </c>
       <c r="E70" s="23"/>
       <c r="F70" s="30"/>
-      <c r="H70" s="66" t="str">
+      <c r="H70" s="40" t="str">
         <f t="shared" si="4"/>
         <v>10,7</v>
       </c>
-      <c r="I70" s="67">
+      <c r="I70" s="41">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
-      <c r="J70" s="68">
+      <c r="J70" s="42">
         <f t="shared" si="6"/>
         <v>3.8</v>
       </c>
@@ -3133,7 +3135,7 @@
         <v>13.4</v>
       </c>
       <c r="C71" s="3"/>
-      <c r="D71" s="41"/>
+      <c r="D71" s="52"/>
       <c r="E71" s="23">
         <v>88</v>
       </c>
@@ -3141,15 +3143,15 @@
         <f t="shared" si="7"/>
         <v>110</v>
       </c>
-      <c r="H71" s="66">
+      <c r="H71" s="40">
         <f t="shared" si="4"/>
         <v>13.4</v>
       </c>
-      <c r="I71" s="67">
+      <c r="I71" s="41">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
-      <c r="J71" s="68">
+      <c r="J71" s="42">
         <f t="shared" si="6"/>
         <v>3.8</v>
       </c>
@@ -3159,7 +3161,7 @@
         <v>20</v>
       </c>
       <c r="C72" s="3"/>
-      <c r="D72" s="42"/>
+      <c r="D72" s="53"/>
       <c r="E72" s="23">
         <v>90</v>
       </c>
@@ -3167,15 +3169,15 @@
         <f t="shared" si="7"/>
         <v>112.5</v>
       </c>
-      <c r="H72" s="66">
+      <c r="H72" s="40">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="I72" s="67">
+      <c r="I72" s="41">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
-      <c r="J72" s="68">
+      <c r="J72" s="42">
         <f t="shared" si="6"/>
         <v>3.8</v>
       </c>
@@ -3187,20 +3189,20 @@
       <c r="C73" s="3">
         <v>204</v>
       </c>
-      <c r="D73" s="40">
+      <c r="D73" s="51">
         <v>4.0999999999999996</v>
       </c>
       <c r="E73" s="23"/>
       <c r="F73" s="30"/>
-      <c r="H73" s="66" t="str">
+      <c r="H73" s="40" t="str">
         <f t="shared" si="4"/>
         <v>10,7</v>
       </c>
-      <c r="I73" s="67">
+      <c r="I73" s="41">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
-      <c r="J73" s="68">
+      <c r="J73" s="42">
         <f t="shared" si="6"/>
         <v>4.0999999999999996</v>
       </c>
@@ -3210,7 +3212,7 @@
         <v>13.4</v>
       </c>
       <c r="C74" s="3"/>
-      <c r="D74" s="41"/>
+      <c r="D74" s="52"/>
       <c r="E74" s="23">
         <v>88</v>
       </c>
@@ -3218,15 +3220,15 @@
         <f t="shared" si="7"/>
         <v>110</v>
       </c>
-      <c r="H74" s="66">
+      <c r="H74" s="40">
         <f t="shared" si="4"/>
         <v>13.4</v>
       </c>
-      <c r="I74" s="67">
+      <c r="I74" s="41">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
-      <c r="J74" s="68">
+      <c r="J74" s="42">
         <f t="shared" si="6"/>
         <v>4.0999999999999996</v>
       </c>
@@ -3236,7 +3238,7 @@
         <v>20</v>
       </c>
       <c r="C75" s="3"/>
-      <c r="D75" s="42"/>
+      <c r="D75" s="53"/>
       <c r="E75" s="23">
         <v>90</v>
       </c>
@@ -3244,15 +3246,15 @@
         <f t="shared" si="7"/>
         <v>112.5</v>
       </c>
-      <c r="H75" s="66">
+      <c r="H75" s="40">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="I75" s="67">
+      <c r="I75" s="41">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
-      <c r="J75" s="68">
+      <c r="J75" s="42">
         <f t="shared" si="6"/>
         <v>4.0999999999999996</v>
       </c>
@@ -3274,15 +3276,15 @@
         <f t="shared" si="7"/>
         <v>112.5</v>
       </c>
-      <c r="H76" s="66" t="str">
+      <c r="H76" s="40" t="str">
         <f t="shared" si="4"/>
         <v>13,4</v>
       </c>
-      <c r="I76" s="67">
+      <c r="I76" s="41">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
-      <c r="J76" s="68">
+      <c r="J76" s="42">
         <f t="shared" si="6"/>
         <v>4.8</v>
       </c>
@@ -3304,21 +3306,32 @@
         <f t="shared" si="7"/>
         <v>116.25</v>
       </c>
-      <c r="H77" s="66">
+      <c r="H77" s="40">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="I77" s="67">
+      <c r="I77" s="41">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
-      <c r="J77" s="68">
+      <c r="J77" s="42">
         <f t="shared" si="6"/>
         <v>5.6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D67:D69"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -3335,17 +3348,6 @@
     <mergeCell ref="D58:D59"/>
     <mergeCell ref="D62:D64"/>
     <mergeCell ref="D70:D72"/>
-    <mergeCell ref="D67:D69"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.31" bottom="0.38" header="0.17" footer="0.3"/>
   <pageSetup paperSize="8" scale="92" orientation="portrait" r:id="rId1"/>
@@ -3356,48 +3358,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="5.875" customWidth="1"/>
     <col min="2" max="4" width="12.75" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="30.875" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="51" t="s">
+      <c r="F1" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="62" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="44"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="57"/>
-      <c r="J2" s="65"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="66"/>
+      <c r="J2" s="48"/>
     </row>
     <row r="3" spans="1:10" ht="15">
       <c r="A3" s="20"/>
@@ -3418,9 +3421,9 @@
         <v>112.5</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="68">
+        <v>33</v>
+      </c>
+      <c r="J3" s="42">
         <f>IF(D3="",J2, IF(ISNUMBER(FIND("-", D3)), LEFT(D3, FIND("-",D3)-1),D3))</f>
         <v>3</v>
       </c>
@@ -3443,7 +3446,7 @@
         <f t="shared" ref="F4:F35" si="0">E4*1.25</f>
         <v>112.5</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="42">
         <f t="shared" ref="J4:J35" si="1">IF(D4="",J3, IF(ISNUMBER(FIND("-", D4)), LEFT(D4, FIND("-",D4)-1),D4))</f>
         <v>3.3</v>
       </c>
@@ -3466,7 +3469,7 @@
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="J5" s="68">
+      <c r="J5" s="42">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -3489,7 +3492,7 @@
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="J6" s="68">
+      <c r="J6" s="42">
         <f t="shared" si="1"/>
         <v>4.0999999999999996</v>
       </c>
@@ -3512,7 +3515,7 @@
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="J7" s="68">
+      <c r="J7" s="42">
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
@@ -3535,7 +3538,7 @@
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="J8" s="68" t="str">
+      <c r="J8" s="42" t="str">
         <f t="shared" si="1"/>
         <v>4,8</v>
       </c>
@@ -3558,7 +3561,7 @@
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="J9" s="68" t="str">
+      <c r="J9" s="42" t="str">
         <f t="shared" si="1"/>
         <v>5,2</v>
       </c>
@@ -3581,7 +3584,7 @@
         <f t="shared" si="0"/>
         <v>116.25</v>
       </c>
-      <c r="J10" s="68" t="str">
+      <c r="J10" s="42" t="str">
         <f t="shared" si="1"/>
         <v>5,2</v>
       </c>
@@ -3604,7 +3607,7 @@
         <f t="shared" si="0"/>
         <v>116.25</v>
       </c>
-      <c r="J11" s="68" t="str">
+      <c r="J11" s="42" t="str">
         <f t="shared" si="1"/>
         <v>5,6</v>
       </c>
@@ -3627,7 +3630,7 @@
         <f t="shared" si="0"/>
         <v>118.75</v>
       </c>
-      <c r="J12" s="68">
+      <c r="J12" s="42">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -3650,7 +3653,7 @@
         <f t="shared" si="0"/>
         <v>122.5</v>
       </c>
-      <c r="J13" s="68" t="str">
+      <c r="J13" s="42" t="str">
         <f t="shared" si="1"/>
         <v>6,2</v>
       </c>
@@ -3673,7 +3676,7 @@
         <f t="shared" si="0"/>
         <v>131.25</v>
       </c>
-      <c r="J14" s="68">
+      <c r="J14" s="42">
         <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
@@ -3696,7 +3699,7 @@
         <f t="shared" si="0"/>
         <v>137.5</v>
       </c>
-      <c r="J15" s="68">
+      <c r="J15" s="42">
         <f t="shared" si="1"/>
         <v>8.1</v>
       </c>
@@ -3719,7 +3722,7 @@
         <f t="shared" si="0"/>
         <v>137.5</v>
       </c>
-      <c r="J16" s="68">
+      <c r="J16" s="42">
         <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
@@ -3742,7 +3745,7 @@
         <f t="shared" si="0"/>
         <v>143.75</v>
       </c>
-      <c r="J17" s="68">
+      <c r="J17" s="42">
         <f t="shared" si="1"/>
         <v>9.1999999999999993</v>
       </c>
@@ -3765,7 +3768,7 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="J18" s="68">
+      <c r="J18" s="42">
         <f t="shared" si="1"/>
         <v>9.8000000000000007</v>
       </c>
@@ -3788,7 +3791,7 @@
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="J19" s="68">
+      <c r="J19" s="42">
         <f t="shared" si="1"/>
         <v>4.3</v>
       </c>
@@ -3811,7 +3814,7 @@
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="J20" s="68">
+      <c r="J20" s="42">
         <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
@@ -3834,7 +3837,7 @@
         <f t="shared" si="0"/>
         <v>131.25</v>
       </c>
-      <c r="J21" s="68">
+      <c r="J21" s="42">
         <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
@@ -3857,7 +3860,7 @@
         <f t="shared" si="0"/>
         <v>137.5</v>
       </c>
-      <c r="J22" s="68">
+      <c r="J22" s="42">
         <f t="shared" si="1"/>
         <v>4.9000000000000004</v>
       </c>
@@ -3880,7 +3883,7 @@
         <f t="shared" si="0"/>
         <v>137.5</v>
       </c>
-      <c r="J23" s="68">
+      <c r="J23" s="42">
         <f t="shared" si="1"/>
         <v>5.2</v>
       </c>
@@ -3903,7 +3906,7 @@
         <f t="shared" si="0"/>
         <v>137.5</v>
       </c>
-      <c r="J24" s="68">
+      <c r="J24" s="42">
         <f t="shared" si="1"/>
         <v>5.65</v>
       </c>
@@ -3926,7 +3929,7 @@
         <f t="shared" si="0"/>
         <v>143.75</v>
       </c>
-      <c r="J25" s="68">
+      <c r="J25" s="42">
         <f t="shared" si="1"/>
         <v>5.65</v>
       </c>
@@ -3949,7 +3952,7 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="J26" s="68">
+      <c r="J26" s="42">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -3972,7 +3975,7 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="J27" s="68">
+      <c r="J27" s="42">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
@@ -3995,7 +3998,7 @@
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="J28" s="68">
+      <c r="J28" s="42">
         <f t="shared" si="1"/>
         <v>4.9000000000000004</v>
       </c>
@@ -4018,7 +4021,7 @@
         <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
-      <c r="J29" s="68">
+      <c r="J29" s="42">
         <f t="shared" si="1"/>
         <v>5.0999999999999996</v>
       </c>
@@ -4041,7 +4044,7 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="J30" s="68">
+      <c r="J30" s="42">
         <f t="shared" si="1"/>
         <v>4.9000000000000004</v>
       </c>
@@ -4064,7 +4067,7 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="J31" s="68">
+      <c r="J31" s="42">
         <f t="shared" si="1"/>
         <v>6.6</v>
       </c>
@@ -4087,7 +4090,7 @@
         <f t="shared" si="0"/>
         <v>118.75</v>
       </c>
-      <c r="J32" s="68">
+      <c r="J32" s="42">
         <f t="shared" si="1"/>
         <v>5.7</v>
       </c>
@@ -4110,7 +4113,7 @@
         <f t="shared" si="0"/>
         <v>143.75</v>
       </c>
-      <c r="J33" s="68">
+      <c r="J33" s="42">
         <f t="shared" si="1"/>
         <v>5.7</v>
       </c>
@@ -4133,7 +4136,7 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="J34" s="68">
+      <c r="J34" s="42">
         <f t="shared" si="1"/>
         <v>5.7</v>
       </c>
@@ -4156,7 +4159,7 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="J35" s="68">
+      <c r="J35" s="42">
         <f t="shared" si="1"/>
         <v>5.7</v>
       </c>

</xml_diff>